<commit_message>
Fixed spelling errors in validation tables.
</commit_message>
<xml_diff>
--- a/test/validation/Scenarios/BloodChemistryValidation.xlsx
+++ b/test/validation/Scenarios/BloodChemistryValidation.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22026"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\Source\engine\test\validation\Scenarios\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A695258E-B118-4A3D-8D5E-951F3E78FD3C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="60" windowWidth="13395" windowHeight="7230"/>
+    <workbookView xWindow="15510" yWindow="7395" windowWidth="32670" windowHeight="23535" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="1" r:id="rId1"/>
@@ -13,12 +19,20 @@
     <sheet name="SalineInfusion" sheetId="5" r:id="rId4"/>
     <sheet name="Nomogram" sheetId="6" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="561" uniqueCount="194">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="561" uniqueCount="193">
   <si>
     <t>|</t>
   </si>
@@ -44,18 +58,12 @@
     <t>Hypo/Hyperventilation</t>
   </si>
   <si>
-    <t>Consious Breathing</t>
-  </si>
-  <si>
     <t>Saline Infusion</t>
   </si>
   <si>
     <t>Infusion of 0.9% Saline</t>
   </si>
   <si>
-    <t>Differentiating between metabolic and respiratory distrubances</t>
-  </si>
-  <si>
     <t>1. Chowdhury, Abeed H. et al. "A Randomized, Controlled, Double-Blind Crossover Study on the Effects of 2-L Infusions of 0.9% Saline and Plasma-Lyte(R) 148 on Renal Blood Flow Velocity and Renal Cortical Tissue Perfusion in Healthy Volunteers," Annals of Surgery, Vol.256, No.1, July 2012, Lippincott</t>
   </si>
   <si>
@@ -99,9 +107,6 @@
   </si>
   <si>
     <t>Partial Pressure CO2 (mmHg)</t>
-  </si>
-  <si>
-    <t>Stong Ion Difference (mmol/L)</t>
   </si>
   <si>
     <t>Base</t>
@@ -717,11 +722,17 @@
   <si>
     <t>Nomogram</t>
   </si>
+  <si>
+    <t>Conscious Breathing</t>
+  </si>
+  <si>
+    <t>Differentiating between metabolic and respiratory disturbances</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="31" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1606,17 +1617,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="46">
@@ -1645,14 +1656,14 @@
     <cellStyle name="Accent5" xfId="34" builtinId="45" customBuiltin="1"/>
     <cellStyle name="Accent6" xfId="38" builtinId="49" customBuiltin="1"/>
     <cellStyle name="Bad" xfId="7" builtinId="27"/>
-    <cellStyle name="Bad 2" xfId="45"/>
-    <cellStyle name="Bad 3" xfId="43"/>
+    <cellStyle name="Bad 2" xfId="45" xr:uid="{00000000-0005-0000-0000-000019000000}"/>
+    <cellStyle name="Bad 3" xfId="43" xr:uid="{00000000-0005-0000-0000-00001A000000}"/>
     <cellStyle name="Calculation" xfId="11" builtinId="22" customBuiltin="1"/>
     <cellStyle name="Check Cell" xfId="13" builtinId="23" customBuiltin="1"/>
     <cellStyle name="Explanatory Text" xfId="16" builtinId="53" customBuiltin="1"/>
     <cellStyle name="Good" xfId="6" builtinId="26"/>
-    <cellStyle name="Good 2" xfId="44"/>
-    <cellStyle name="Good 3" xfId="42"/>
+    <cellStyle name="Good 2" xfId="44" xr:uid="{00000000-0005-0000-0000-00001F000000}"/>
+    <cellStyle name="Good 3" xfId="42" xr:uid="{00000000-0005-0000-0000-000020000000}"/>
     <cellStyle name="Heading 1" xfId="2" builtinId="16" customBuiltin="1"/>
     <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
     <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
@@ -1672,6 +1683,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -1720,7 +1734,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1753,9 +1767,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1788,6 +1819,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1963,11 +2011,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="P2" sqref="P2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2003,19 +2051,19 @@
         <v>0</v>
       </c>
       <c r="F1" s="24" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="G1" s="24" t="s">
         <v>0</v>
       </c>
       <c r="H1" s="24" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="I1" s="24" t="s">
         <v>0</v>
       </c>
       <c r="J1" s="24" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="K1" s="24" t="s">
         <v>0</v>
@@ -2035,25 +2083,25 @@
         <v>3</v>
       </c>
       <c r="E2" s="25" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="F2" s="23" t="s">
         <v>3</v>
       </c>
       <c r="G2" s="25" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="H2" s="23" t="s">
         <v>3</v>
       </c>
       <c r="I2" s="25" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="J2" s="23" t="s">
         <v>3</v>
       </c>
       <c r="K2" s="25" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.2">
@@ -2067,28 +2115,28 @@
         <v>0</v>
       </c>
       <c r="D3" s="26" t="s">
-        <v>8</v>
+        <v>191</v>
       </c>
       <c r="E3" s="25" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="F3" s="34">
         <v>0</v>
       </c>
       <c r="G3" s="25" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="H3" s="35">
         <v>0</v>
       </c>
       <c r="I3" s="25" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="J3" s="33">
         <v>0</v>
       </c>
       <c r="K3" s="25" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.2">
@@ -2096,34 +2144,34 @@
         <v>0</v>
       </c>
       <c r="B4" s="29" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" s="29" t="s">
+        <v>0</v>
+      </c>
+      <c r="D4" s="26" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="29" t="s">
-        <v>0</v>
-      </c>
-      <c r="D4" s="26" t="s">
-        <v>10</v>
-      </c>
       <c r="E4" s="25" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="F4" s="34">
         <v>0</v>
       </c>
       <c r="G4" s="25" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="H4" s="35">
         <v>0</v>
       </c>
       <c r="I4" s="25" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="J4" s="33">
         <v>0</v>
       </c>
       <c r="K4" s="25" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
     </row>
     <row r="5" spans="1:11" ht="25.5" x14ac:dyDescent="0.2">
@@ -2131,34 +2179,34 @@
         <v>0</v>
       </c>
       <c r="B5" s="29" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="C5" s="29" t="s">
         <v>0</v>
       </c>
       <c r="D5" s="26" t="s">
-        <v>11</v>
+        <v>192</v>
       </c>
       <c r="E5" s="25" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="F5" s="34">
         <v>0</v>
       </c>
       <c r="G5" s="25" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="H5" s="35">
         <v>0</v>
       </c>
       <c r="I5" s="25" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="J5" s="33">
         <v>0</v>
       </c>
       <c r="K5" s="25" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.2">
@@ -2166,7 +2214,7 @@
         <v>0</v>
       </c>
       <c r="B6" s="31" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="C6" s="31"/>
       <c r="D6" s="30"/>
@@ -2189,7 +2237,7 @@
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B8" s="32" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D8" s="37" t="s">
         <v>6</v>
@@ -2197,51 +2245,51 @@
     </row>
     <row r="9" spans="1:11" ht="76.5" x14ac:dyDescent="0.2">
       <c r="D9" s="38" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="10" spans="1:11" ht="38.25" x14ac:dyDescent="0.2">
       <c r="B10" s="39"/>
       <c r="D10" s="38" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="G10" s="39"/>
     </row>
     <row r="11" spans="1:11" ht="51" x14ac:dyDescent="0.2">
       <c r="B11" s="39"/>
       <c r="D11" s="38" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="G11" s="40"/>
     </row>
     <row r="12" spans="1:11" ht="38.25" x14ac:dyDescent="0.2">
       <c r="B12" s="39"/>
       <c r="D12" s="38" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="G12" s="40"/>
     </row>
     <row r="13" spans="1:11" ht="38.25" x14ac:dyDescent="0.2">
       <c r="B13" s="39"/>
       <c r="D13" s="38" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="G13" s="40"/>
     </row>
     <row r="14" spans="1:11" ht="76.5" x14ac:dyDescent="0.2">
       <c r="B14" s="39"/>
       <c r="D14" s="38" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="15" spans="1:11" ht="38.25" x14ac:dyDescent="0.2">
       <c r="D15" s="38" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="16" spans="1:11" ht="76.5" x14ac:dyDescent="0.2">
       <c r="D16" s="38" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="17" spans="4:4" x14ac:dyDescent="0.2">
@@ -2253,11 +2301,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="P2" sqref="P2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2272,7 +2320,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="21" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="C1" s="19" t="s">
         <v>0</v>
@@ -2291,35 +2339,35 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="19" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="B3" s="17" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="C3" s="19" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="19" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="B4" s="18" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="C4" s="19" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="19" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="B5" s="16" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="C5" s="19" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
     </row>
   </sheetData>
@@ -2328,11 +2376,11 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:Q7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J7" sqref="J7"/>
+    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
+      <selection activeCell="P2" sqref="P2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2361,7 +2409,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="60" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C2" s="63" t="s">
         <v>0</v>
@@ -2373,7 +2421,7 @@
         <v>0</v>
       </c>
       <c r="F2" s="60" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="G2" s="63" t="s">
         <v>0</v>
@@ -2385,25 +2433,25 @@
         <v>0</v>
       </c>
       <c r="J2" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="K2" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="M2" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="N2" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="K2" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="L2" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="M2" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="N2" s="1" t="s">
-        <v>26</v>
-      </c>
       <c r="O2" s="6" t="s">
         <v>0</v>
       </c>
       <c r="P2" s="1" t="s">
-        <v>27</v>
+        <v>45</v>
       </c>
       <c r="Q2" s="6" t="s">
         <v>0</v>
@@ -2467,52 +2515,52 @@
         <v>0</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="C4" s="63" t="s">
         <v>0</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="E4" s="63" t="s">
         <v>0</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="G4" s="63" t="s">
         <v>0</v>
       </c>
       <c r="H4" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="I4" s="62" t="s">
+        <v>95</v>
+      </c>
+      <c r="J4" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="K4" s="65" t="s">
+        <v>114</v>
+      </c>
+      <c r="L4" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="M4" s="65" t="s">
+        <v>114</v>
+      </c>
+      <c r="N4" s="4" t="s">
         <v>118</v>
       </c>
-      <c r="I4" s="62" t="s">
-        <v>98</v>
-      </c>
-      <c r="J4" s="4" t="s">
-        <v>119</v>
-      </c>
-      <c r="K4" s="65" t="s">
-        <v>117</v>
-      </c>
-      <c r="L4" s="4" t="s">
-        <v>120</v>
-      </c>
-      <c r="M4" s="65" t="s">
-        <v>117</v>
-      </c>
-      <c r="N4" s="4" t="s">
-        <v>121</v>
-      </c>
       <c r="O4" s="65" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="P4" s="4" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="Q4" s="65" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.25">
@@ -2520,105 +2568,105 @@
         <v>0</v>
       </c>
       <c r="B5" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="C5" s="63" t="s">
+        <v>0</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E5" s="63" t="s">
+        <v>0</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="G5" s="63" t="s">
+        <v>0</v>
+      </c>
+      <c r="H5" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="I5" s="62" t="s">
+        <v>109</v>
+      </c>
+      <c r="J5" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="K5" s="65" t="s">
+        <v>114</v>
+      </c>
+      <c r="L5" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="M5" s="65" t="s">
+        <v>114</v>
+      </c>
+      <c r="N5" s="4" t="s">
+        <v>124</v>
+      </c>
+      <c r="O5" s="65" t="s">
+        <v>114</v>
+      </c>
+      <c r="P5" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="Q5" s="65" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" ht="30" x14ac:dyDescent="0.25">
+      <c r="A6" s="63" t="s">
+        <v>0</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="C6" s="63" t="s">
+        <v>0</v>
+      </c>
+      <c r="D6" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C5" s="63" t="s">
-        <v>0</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="E5" s="63" t="s">
-        <v>0</v>
-      </c>
-      <c r="F5" s="4" t="s">
-        <v>114</v>
-      </c>
-      <c r="G5" s="63" t="s">
-        <v>0</v>
-      </c>
-      <c r="H5" s="4" t="s">
-        <v>122</v>
-      </c>
-      <c r="I5" s="62" t="s">
+      <c r="E6" s="63" t="s">
+        <v>0</v>
+      </c>
+      <c r="F6" s="4" t="s">
         <v>112</v>
       </c>
-      <c r="J5" s="4" t="s">
-        <v>125</v>
-      </c>
-      <c r="K5" s="65" t="s">
+      <c r="G6" s="63" t="s">
+        <v>0</v>
+      </c>
+      <c r="H6" s="4" t="s">
+        <v>120</v>
+      </c>
+      <c r="I6" s="62" t="s">
+        <v>95</v>
+      </c>
+      <c r="J6" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="K6" s="65" t="s">
+        <v>114</v>
+      </c>
+      <c r="L6" s="4" t="s">
         <v>117</v>
       </c>
-      <c r="L5" s="4" t="s">
+      <c r="M6" s="65" t="s">
+        <v>114</v>
+      </c>
+      <c r="N6" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="O6" s="65" t="s">
+        <v>114</v>
+      </c>
+      <c r="P6" s="2" t="s">
         <v>126</v>
       </c>
-      <c r="M5" s="65" t="s">
-        <v>117</v>
-      </c>
-      <c r="N5" s="4" t="s">
-        <v>127</v>
-      </c>
-      <c r="O5" s="65" t="s">
-        <v>117</v>
-      </c>
-      <c r="P5" s="4" t="s">
-        <v>129</v>
-      </c>
-      <c r="Q5" s="65" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A6" s="63" t="s">
-        <v>0</v>
-      </c>
-      <c r="B6" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="C6" s="63" t="s">
-        <v>0</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="E6" s="63" t="s">
-        <v>0</v>
-      </c>
-      <c r="F6" s="4" t="s">
-        <v>115</v>
-      </c>
-      <c r="G6" s="63" t="s">
-        <v>0</v>
-      </c>
-      <c r="H6" s="4" t="s">
-        <v>123</v>
-      </c>
-      <c r="I6" s="62" t="s">
-        <v>98</v>
-      </c>
-      <c r="J6" s="4" t="s">
-        <v>119</v>
-      </c>
-      <c r="K6" s="65" t="s">
-        <v>117</v>
-      </c>
-      <c r="L6" s="4" t="s">
-        <v>120</v>
-      </c>
-      <c r="M6" s="65" t="s">
-        <v>117</v>
-      </c>
-      <c r="N6" s="4" t="s">
-        <v>121</v>
-      </c>
-      <c r="O6" s="65" t="s">
-        <v>117</v>
-      </c>
-      <c r="P6" s="2" t="s">
-        <v>129</v>
-      </c>
       <c r="Q6" s="65" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.25">
@@ -2626,52 +2674,52 @@
         <v>0</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="C7" s="63" t="s">
         <v>0</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="E7" s="63" t="s">
         <v>0</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="G7" s="63" t="s">
         <v>0</v>
       </c>
       <c r="H7" s="4" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="I7" s="62" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="J7" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="K7" s="65" t="s">
+        <v>114</v>
+      </c>
+      <c r="L7" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="M7" s="65" t="s">
+        <v>114</v>
+      </c>
+      <c r="N7" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="O7" s="65" t="s">
+        <v>114</v>
+      </c>
+      <c r="P7" s="4" t="s">
         <v>126</v>
       </c>
-      <c r="K7" s="65" t="s">
-        <v>117</v>
-      </c>
-      <c r="L7" s="4" t="s">
-        <v>128</v>
-      </c>
-      <c r="M7" s="65" t="s">
-        <v>117</v>
-      </c>
-      <c r="N7" s="4" t="s">
-        <v>125</v>
-      </c>
-      <c r="O7" s="65" t="s">
-        <v>117</v>
-      </c>
-      <c r="P7" s="4" t="s">
-        <v>129</v>
-      </c>
       <c r="Q7" s="65" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
     </row>
   </sheetData>
@@ -2680,11 +2728,11 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A2:AI10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+    <sheetView tabSelected="1" topLeftCell="AB1" workbookViewId="0">
+      <selection activeCell="P2" sqref="P2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2732,7 +2780,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="42" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C2" s="36" t="s">
         <v>0</v>
@@ -2744,91 +2792,91 @@
         <v>0</v>
       </c>
       <c r="F2" s="42" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="G2" s="36" t="s">
         <v>0</v>
       </c>
       <c r="H2" s="42" t="s">
+        <v>21</v>
+      </c>
+      <c r="I2" s="42" t="s">
+        <v>0</v>
+      </c>
+      <c r="J2" s="42" t="s">
+        <v>34</v>
+      </c>
+      <c r="K2" s="50" t="s">
+        <v>0</v>
+      </c>
+      <c r="L2" s="42" t="s">
+        <v>35</v>
+      </c>
+      <c r="M2" s="50" t="s">
+        <v>0</v>
+      </c>
+      <c r="N2" s="42" t="s">
+        <v>36</v>
+      </c>
+      <c r="O2" s="50" t="s">
+        <v>0</v>
+      </c>
+      <c r="P2" s="42" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q2" s="50" t="s">
+        <v>0</v>
+      </c>
+      <c r="R2" s="42" t="s">
+        <v>38</v>
+      </c>
+      <c r="S2" s="50" t="s">
+        <v>0</v>
+      </c>
+      <c r="T2" s="42" t="s">
+        <v>39</v>
+      </c>
+      <c r="U2" s="50" t="s">
+        <v>0</v>
+      </c>
+      <c r="V2" s="42" t="s">
+        <v>40</v>
+      </c>
+      <c r="W2" s="50" t="s">
+        <v>0</v>
+      </c>
+      <c r="X2" s="42" t="s">
+        <v>41</v>
+      </c>
+      <c r="Y2" s="50" t="s">
+        <v>0</v>
+      </c>
+      <c r="Z2" s="42" t="s">
+        <v>42</v>
+      </c>
+      <c r="AA2" s="50" t="s">
+        <v>0</v>
+      </c>
+      <c r="AB2" s="42" t="s">
+        <v>43</v>
+      </c>
+      <c r="AC2" s="50" t="s">
+        <v>0</v>
+      </c>
+      <c r="AD2" s="42" t="s">
         <v>23</v>
       </c>
-      <c r="I2" s="42" t="s">
-        <v>0</v>
-      </c>
-      <c r="J2" s="42" t="s">
-        <v>37</v>
-      </c>
-      <c r="K2" s="50" t="s">
-        <v>0</v>
-      </c>
-      <c r="L2" s="42" t="s">
-        <v>38</v>
-      </c>
-      <c r="M2" s="50" t="s">
-        <v>0</v>
-      </c>
-      <c r="N2" s="42" t="s">
-        <v>39</v>
-      </c>
-      <c r="O2" s="50" t="s">
-        <v>0</v>
-      </c>
-      <c r="P2" s="42" t="s">
-        <v>40</v>
-      </c>
-      <c r="Q2" s="50" t="s">
-        <v>0</v>
-      </c>
-      <c r="R2" s="42" t="s">
-        <v>41</v>
-      </c>
-      <c r="S2" s="50" t="s">
-        <v>0</v>
-      </c>
-      <c r="T2" s="42" t="s">
-        <v>42</v>
-      </c>
-      <c r="U2" s="50" t="s">
-        <v>0</v>
-      </c>
-      <c r="V2" s="42" t="s">
-        <v>43</v>
-      </c>
-      <c r="W2" s="50" t="s">
-        <v>0</v>
-      </c>
-      <c r="X2" s="42" t="s">
+      <c r="AE2" s="50" t="s">
+        <v>0</v>
+      </c>
+      <c r="AF2" s="42" t="s">
         <v>44</v>
       </c>
-      <c r="Y2" s="50" t="s">
-        <v>0</v>
-      </c>
-      <c r="Z2" s="42" t="s">
+      <c r="AG2" s="50" t="s">
+        <v>0</v>
+      </c>
+      <c r="AH2" s="42" t="s">
         <v>45</v>
-      </c>
-      <c r="AA2" s="50" t="s">
-        <v>0</v>
-      </c>
-      <c r="AB2" s="42" t="s">
-        <v>46</v>
-      </c>
-      <c r="AC2" s="50" t="s">
-        <v>0</v>
-      </c>
-      <c r="AD2" s="42" t="s">
-        <v>25</v>
-      </c>
-      <c r="AE2" s="50" t="s">
-        <v>0</v>
-      </c>
-      <c r="AF2" s="42" t="s">
-        <v>47</v>
-      </c>
-      <c r="AG2" s="50" t="s">
-        <v>0</v>
-      </c>
-      <c r="AH2" s="42" t="s">
-        <v>48</v>
       </c>
       <c r="AI2" s="36" t="s">
         <v>0</v>
@@ -2946,19 +2994,19 @@
         <v>0</v>
       </c>
       <c r="B4" s="51" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="C4" s="69" t="s">
         <v>0</v>
       </c>
       <c r="D4" s="51" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="E4" s="69" t="s">
         <v>0</v>
       </c>
       <c r="F4" s="55" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="G4" s="69" t="s">
         <v>0</v>
@@ -2967,82 +3015,82 @@
         <v>0.5</v>
       </c>
       <c r="I4" s="69" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="J4" s="55" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="K4" s="69" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="L4" s="58">
         <v>0</v>
       </c>
       <c r="M4" s="69" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="N4" s="58" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="O4" s="69" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="P4" s="58" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="Q4" s="69" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="R4" s="58" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="S4" s="69" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="T4" s="58" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="U4" s="69" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="V4" s="58" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="W4" s="69" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="X4" s="58" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="Y4" s="69" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="Z4" s="58" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="AA4" s="69" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="AB4" s="58" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="AC4" s="69" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="AD4" s="58" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="AE4" s="69" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="AF4" s="58" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="AG4" s="69" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="AH4" s="58" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="AI4" s="69" t="s">
         <v>0</v>
@@ -3053,19 +3101,19 @@
         <v>0</v>
       </c>
       <c r="B5" s="51" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="C5" s="57" t="s">
         <v>0</v>
       </c>
       <c r="D5" s="51" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="E5" s="57" t="s">
         <v>0</v>
       </c>
       <c r="F5" s="55" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="G5" s="57" t="s">
         <v>0</v>
@@ -3074,82 +3122,82 @@
         <v>60.5</v>
       </c>
       <c r="I5" s="69" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="J5" s="55" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="K5" s="69" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="L5" s="58" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="M5" s="69" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="N5" s="58" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="O5" s="69" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="P5" s="58" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="Q5" s="69" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="R5" s="58" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="S5" s="69" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="T5" s="58" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="U5" s="69" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="V5" s="58" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="W5" s="69" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="X5" s="58" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="Y5" s="69" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="Z5" s="58" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="AA5" s="69" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="AB5" s="58" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="AC5" s="69" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="AD5" s="58" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="AE5" s="69" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="AF5" s="58" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="AG5" s="69" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="AH5" s="55" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="AI5" s="57" t="s">
         <v>0</v>
@@ -3160,19 +3208,19 @@
         <v>0</v>
       </c>
       <c r="B6" s="51" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C6" s="57" t="s">
         <v>0</v>
       </c>
       <c r="D6" s="51" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="E6" s="57" t="s">
         <v>0</v>
       </c>
       <c r="F6" s="55" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="G6" s="57" t="s">
         <v>0</v>
@@ -3181,82 +3229,82 @@
         <v>90.5</v>
       </c>
       <c r="I6" s="69" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="J6" s="55" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="K6" s="69" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="L6" s="58" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="M6" s="69" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="N6" s="58" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="O6" s="69" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="P6" s="58" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="Q6" s="69" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="R6" s="58" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="S6" s="69" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="T6" s="58" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="U6" s="69" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="V6" s="58" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="W6" s="69" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="X6" s="58" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="Y6" s="69" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="Z6" s="58" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="AA6" s="69" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="AB6" s="58" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="AC6" s="69" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="AD6" s="58" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="AE6" s="69" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="AF6" s="58" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="AG6" s="69" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="AH6" s="58" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="AI6" s="57" t="s">
         <v>0</v>
@@ -3267,19 +3315,19 @@
         <v>0</v>
       </c>
       <c r="B7" s="51" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C7" s="57" t="s">
         <v>0</v>
       </c>
       <c r="D7" s="51" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="E7" s="57" t="s">
         <v>0</v>
       </c>
       <c r="F7" s="55" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="G7" s="57" t="s">
         <v>0</v>
@@ -3288,82 +3336,82 @@
         <v>120.5</v>
       </c>
       <c r="I7" s="69" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="J7" s="55" t="s">
+        <v>54</v>
+      </c>
+      <c r="K7" s="69" t="s">
+        <v>114</v>
+      </c>
+      <c r="L7" s="58" t="s">
+        <v>129</v>
+      </c>
+      <c r="M7" s="69" t="s">
+        <v>114</v>
+      </c>
+      <c r="N7" s="58" t="s">
+        <v>186</v>
+      </c>
+      <c r="O7" s="69" t="s">
+        <v>114</v>
+      </c>
+      <c r="P7" s="58" t="s">
         <v>57</v>
       </c>
-      <c r="K7" s="69" t="s">
-        <v>117</v>
-      </c>
-      <c r="L7" s="58" t="s">
-        <v>132</v>
-      </c>
-      <c r="M7" s="69" t="s">
-        <v>117</v>
-      </c>
-      <c r="N7" s="58" t="s">
-        <v>189</v>
-      </c>
-      <c r="O7" s="69" t="s">
-        <v>117</v>
-      </c>
-      <c r="P7" s="58" t="s">
-        <v>60</v>
-      </c>
       <c r="Q7" s="69" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="R7" s="58" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="S7" s="69" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="T7" s="58" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="U7" s="69" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="V7" s="58" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="W7" s="69" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="X7" s="58" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="Y7" s="69" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="Z7" s="58" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="AA7" s="69" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="AB7" s="58" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="AC7" s="69" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="AD7" s="58" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="AE7" s="69" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="AF7" s="58" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="AG7" s="69" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="AH7" s="58" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="AI7" s="57" t="s">
         <v>0</v>
@@ -3374,19 +3422,19 @@
         <v>0</v>
       </c>
       <c r="B8" s="51" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C8" s="57" t="s">
         <v>0</v>
       </c>
       <c r="D8" s="51" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="E8" s="57" t="s">
         <v>0</v>
       </c>
       <c r="F8" s="48" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="G8" s="57" t="s">
         <v>0</v>
@@ -3395,82 +3443,82 @@
         <v>180.5</v>
       </c>
       <c r="I8" s="69" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="J8" s="55" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="K8" s="69" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="L8" s="58" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="M8" s="69" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="N8" s="58" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="O8" s="69" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="P8" s="58" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="Q8" s="69" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="R8" s="58" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="S8" s="69" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="T8" s="58" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="U8" s="69" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="V8" s="58" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="W8" s="69" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="X8" s="58" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="Y8" s="69" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="Z8" s="58" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="AA8" s="69" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="AB8" s="58" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="AC8" s="69" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="AD8" s="58" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="AE8" s="69" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="AF8" s="58" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="AG8" s="69" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="AH8" s="58" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="AI8" s="57" t="s">
         <v>0</v>
@@ -3481,19 +3529,19 @@
         <v>0</v>
       </c>
       <c r="B9" s="51" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C9" s="57" t="s">
         <v>0</v>
       </c>
       <c r="D9" s="51" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="E9" s="57" t="s">
         <v>0</v>
       </c>
       <c r="F9" s="48" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="G9" s="57" t="s">
         <v>0</v>
@@ -3502,82 +3550,82 @@
         <v>240.5</v>
       </c>
       <c r="I9" s="69" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="J9" s="55" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="K9" s="69" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="L9" s="58" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="M9" s="69" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="N9" s="58" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="O9" s="69" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="P9" s="58" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="Q9" s="69" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="R9" s="58" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="S9" s="69" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="T9" s="58" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="U9" s="69" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="V9" s="58" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="W9" s="69" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="X9" s="58" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="Y9" s="69" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="Z9" s="58" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="AA9" s="69" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="AB9" s="58" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="AC9" s="69" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="AD9" s="58" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="AE9" s="69" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="AF9" s="58" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="AG9" s="69" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="AH9" s="58" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="AI9" s="57" t="s">
         <v>0</v>
@@ -3624,11 +3672,11 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:H25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D32" sqref="D32"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="P2" sqref="P2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3643,11 +3691,11 @@
   <sheetData>
     <row r="1" spans="2:8" s="67" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:8" ht="18" x14ac:dyDescent="0.25">
-      <c r="B2" s="73" t="s">
-        <v>65</v>
+      <c r="B2" s="72" t="s">
+        <v>62</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="D2" s="70">
         <v>20</v>
@@ -3666,75 +3714,75 @@
       </c>
     </row>
     <row r="3" spans="2:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="74"/>
+      <c r="B3" s="73"/>
       <c r="C3" s="9" t="s">
-        <v>67</v>
-      </c>
-      <c r="D3" s="72"/>
-      <c r="E3" s="72"/>
-      <c r="F3" s="72"/>
-      <c r="G3" s="72"/>
-      <c r="H3" s="72"/>
+        <v>64</v>
+      </c>
+      <c r="D3" s="71"/>
+      <c r="E3" s="71"/>
+      <c r="F3" s="71"/>
+      <c r="G3" s="71"/>
+      <c r="H3" s="71"/>
     </row>
     <row r="4" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B4" s="70">
         <v>38</v>
       </c>
       <c r="C4" s="70" t="s">
+        <v>65</v>
+      </c>
+      <c r="D4" s="10" t="s">
+        <v>66</v>
+      </c>
+      <c r="E4" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="F4" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="G4" s="12" t="s">
         <v>68</v>
       </c>
-      <c r="D4" s="10" t="s">
+      <c r="H4" s="12" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="5" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B5" s="74"/>
+      <c r="C5" s="74"/>
+      <c r="D5" s="10" t="s">
         <v>69</v>
       </c>
-      <c r="E4" s="12" t="s">
+      <c r="E5" s="12" t="s">
+        <v>69</v>
+      </c>
+      <c r="F5" s="12" t="s">
+        <v>69</v>
+      </c>
+      <c r="G5" s="12" t="s">
+        <v>69</v>
+      </c>
+      <c r="H5" s="12" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="6" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B6" s="71"/>
+      <c r="C6" s="71"/>
+      <c r="D6" s="11" t="s">
         <v>70</v>
       </c>
-      <c r="F4" s="12" t="s">
-        <v>70</v>
-      </c>
-      <c r="G4" s="12" t="s">
+      <c r="E6" s="13" t="s">
         <v>71</v>
       </c>
-      <c r="H4" s="12" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="5" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B5" s="71"/>
-      <c r="C5" s="71"/>
-      <c r="D5" s="10" t="s">
+      <c r="F6" s="13" t="s">
         <v>72</v>
       </c>
-      <c r="E5" s="12" t="s">
-        <v>72</v>
-      </c>
-      <c r="F5" s="12" t="s">
-        <v>72</v>
-      </c>
-      <c r="G5" s="12" t="s">
-        <v>72</v>
-      </c>
-      <c r="H5" s="12" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="6" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="72"/>
-      <c r="C6" s="72"/>
-      <c r="D6" s="11" t="s">
+      <c r="G6" s="13" t="s">
         <v>73</v>
       </c>
-      <c r="E6" s="13" t="s">
-        <v>74</v>
-      </c>
-      <c r="F6" s="13" t="s">
-        <v>75</v>
-      </c>
-      <c r="G6" s="13" t="s">
-        <v>76</v>
-      </c>
       <c r="H6" s="13" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
     </row>
     <row r="7" spans="2:8" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3742,79 +3790,79 @@
         <v>38</v>
       </c>
       <c r="C7" s="70" t="s">
+        <v>74</v>
+      </c>
+      <c r="D7" s="11" t="s">
+        <v>75</v>
+      </c>
+      <c r="E7" s="11" t="s">
+        <v>75</v>
+      </c>
+      <c r="F7" s="11" t="s">
+        <v>75</v>
+      </c>
+      <c r="G7" s="11" t="s">
+        <v>75</v>
+      </c>
+      <c r="H7" s="11" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="8" spans="2:8" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B8" s="74"/>
+      <c r="C8" s="74"/>
+      <c r="D8" s="11" t="s">
+        <v>76</v>
+      </c>
+      <c r="E8" s="11" t="s">
+        <v>76</v>
+      </c>
+      <c r="F8" s="11" t="s">
+        <v>76</v>
+      </c>
+      <c r="G8" s="11" t="s">
+        <v>76</v>
+      </c>
+      <c r="H8" s="11" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="9" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B9" s="74"/>
+      <c r="C9" s="74"/>
+      <c r="D9" s="11" t="s">
         <v>77</v>
       </c>
-      <c r="D7" s="11" t="s">
+      <c r="E9" s="11" t="s">
+        <v>77</v>
+      </c>
+      <c r="F9" s="11" t="s">
+        <v>77</v>
+      </c>
+      <c r="G9" s="11" t="s">
+        <v>77</v>
+      </c>
+      <c r="H9" s="11" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="10" spans="2:8" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B10" s="71"/>
+      <c r="C10" s="71"/>
+      <c r="D10" s="11" t="s">
         <v>78</v>
       </c>
-      <c r="E7" s="11" t="s">
+      <c r="E10" s="11" t="s">
         <v>78</v>
       </c>
-      <c r="F7" s="11" t="s">
+      <c r="F10" s="11" t="s">
         <v>78</v>
       </c>
-      <c r="G7" s="11" t="s">
-        <v>78</v>
-      </c>
-      <c r="H7" s="11" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="8" spans="2:8" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="71"/>
-      <c r="C8" s="71"/>
-      <c r="D8" s="11" t="s">
+      <c r="G10" s="11" t="s">
         <v>79</v>
       </c>
-      <c r="E8" s="11" t="s">
+      <c r="H10" s="11" t="s">
         <v>79</v>
-      </c>
-      <c r="F8" s="11" t="s">
-        <v>79</v>
-      </c>
-      <c r="G8" s="11" t="s">
-        <v>79</v>
-      </c>
-      <c r="H8" s="11" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="9" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="71"/>
-      <c r="C9" s="71"/>
-      <c r="D9" s="11" t="s">
-        <v>80</v>
-      </c>
-      <c r="E9" s="11" t="s">
-        <v>80</v>
-      </c>
-      <c r="F9" s="11" t="s">
-        <v>80</v>
-      </c>
-      <c r="G9" s="11" t="s">
-        <v>80</v>
-      </c>
-      <c r="H9" s="11" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="10" spans="2:8" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="72"/>
-      <c r="C10" s="72"/>
-      <c r="D10" s="11" t="s">
-        <v>81</v>
-      </c>
-      <c r="E10" s="11" t="s">
-        <v>81</v>
-      </c>
-      <c r="F10" s="11" t="s">
-        <v>81</v>
-      </c>
-      <c r="G10" s="11" t="s">
-        <v>82</v>
-      </c>
-      <c r="H10" s="11" t="s">
-        <v>82</v>
       </c>
     </row>
     <row r="11" spans="2:8" x14ac:dyDescent="0.25">
@@ -3822,56 +3870,56 @@
         <v>41</v>
       </c>
       <c r="C11" s="70" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="D11" s="12" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="E11" s="12" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="F11" s="12" t="s">
+        <v>80</v>
+      </c>
+      <c r="G11" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="H11" s="12" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="12" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B12" s="74"/>
+      <c r="C12" s="74"/>
+      <c r="D12" s="12" t="s">
+        <v>81</v>
+      </c>
+      <c r="E12" s="12" t="s">
+        <v>81</v>
+      </c>
+      <c r="F12" s="12" t="s">
+        <v>82</v>
+      </c>
+      <c r="G12" s="12" t="s">
         <v>83</v>
       </c>
-      <c r="G11" s="12" t="s">
-        <v>70</v>
-      </c>
-      <c r="H11" s="12" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="12" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B12" s="71"/>
-      <c r="C12" s="71"/>
-      <c r="D12" s="12" t="s">
-        <v>84</v>
-      </c>
-      <c r="E12" s="12" t="s">
-        <v>84</v>
-      </c>
-      <c r="F12" s="12" t="s">
-        <v>85</v>
-      </c>
-      <c r="G12" s="12" t="s">
-        <v>86</v>
-      </c>
       <c r="H12" s="12" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
     </row>
     <row r="13" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="72"/>
-      <c r="C13" s="72"/>
+      <c r="B13" s="71"/>
+      <c r="C13" s="71"/>
       <c r="D13" s="14"/>
       <c r="E13" s="14"/>
       <c r="F13" s="13" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="G13" s="13" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="H13" s="13" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
     </row>
     <row r="14" spans="2:8" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3879,79 +3927,79 @@
         <v>41</v>
       </c>
       <c r="C14" s="70" t="s">
+        <v>74</v>
+      </c>
+      <c r="D14" s="11" t="s">
+        <v>75</v>
+      </c>
+      <c r="E14" s="11" t="s">
+        <v>75</v>
+      </c>
+      <c r="F14" s="11" t="s">
+        <v>75</v>
+      </c>
+      <c r="G14" s="11" t="s">
+        <v>75</v>
+      </c>
+      <c r="H14" s="11" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="15" spans="2:8" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B15" s="74"/>
+      <c r="C15" s="74"/>
+      <c r="D15" s="11" t="s">
+        <v>76</v>
+      </c>
+      <c r="E15" s="11" t="s">
+        <v>76</v>
+      </c>
+      <c r="F15" s="11" t="s">
+        <v>76</v>
+      </c>
+      <c r="G15" s="11" t="s">
+        <v>76</v>
+      </c>
+      <c r="H15" s="11" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="16" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B16" s="74"/>
+      <c r="C16" s="74"/>
+      <c r="D16" s="11" t="s">
         <v>77</v>
       </c>
-      <c r="D14" s="11" t="s">
+      <c r="E16" s="11" t="s">
+        <v>77</v>
+      </c>
+      <c r="F16" s="11" t="s">
+        <v>77</v>
+      </c>
+      <c r="G16" s="11" t="s">
+        <v>77</v>
+      </c>
+      <c r="H16" s="11" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="17" spans="2:8" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B17" s="71"/>
+      <c r="C17" s="71"/>
+      <c r="D17" s="11" t="s">
+        <v>79</v>
+      </c>
+      <c r="E17" s="11" t="s">
         <v>78</v>
       </c>
-      <c r="E14" s="11" t="s">
+      <c r="F17" s="11" t="s">
         <v>78</v>
       </c>
-      <c r="F14" s="11" t="s">
-        <v>78</v>
-      </c>
-      <c r="G14" s="11" t="s">
-        <v>78</v>
-      </c>
-      <c r="H14" s="11" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="15" spans="2:8" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="71"/>
-      <c r="C15" s="71"/>
-      <c r="D15" s="11" t="s">
+      <c r="G17" s="11" t="s">
         <v>79</v>
       </c>
-      <c r="E15" s="11" t="s">
+      <c r="H17" s="11" t="s">
         <v>79</v>
-      </c>
-      <c r="F15" s="11" t="s">
-        <v>79</v>
-      </c>
-      <c r="G15" s="11" t="s">
-        <v>79</v>
-      </c>
-      <c r="H15" s="11" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="16" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="71"/>
-      <c r="C16" s="71"/>
-      <c r="D16" s="11" t="s">
-        <v>80</v>
-      </c>
-      <c r="E16" s="11" t="s">
-        <v>80</v>
-      </c>
-      <c r="F16" s="11" t="s">
-        <v>80</v>
-      </c>
-      <c r="G16" s="11" t="s">
-        <v>80</v>
-      </c>
-      <c r="H16" s="11" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="17" spans="2:8" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="72"/>
-      <c r="C17" s="72"/>
-      <c r="D17" s="11" t="s">
-        <v>82</v>
-      </c>
-      <c r="E17" s="11" t="s">
-        <v>81</v>
-      </c>
-      <c r="F17" s="11" t="s">
-        <v>81</v>
-      </c>
-      <c r="G17" s="11" t="s">
-        <v>82</v>
-      </c>
-      <c r="H17" s="11" t="s">
-        <v>82</v>
       </c>
     </row>
     <row r="18" spans="2:8" x14ac:dyDescent="0.25">
@@ -3959,60 +4007,60 @@
         <v>44</v>
       </c>
       <c r="C18" s="70" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="D18" s="12" t="s">
+        <v>86</v>
+      </c>
+      <c r="E18" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="F18" s="12" t="s">
+        <v>87</v>
+      </c>
+      <c r="G18" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="H18" s="12" t="s">
         <v>89</v>
       </c>
-      <c r="E18" s="12" t="s">
-        <v>69</v>
-      </c>
-      <c r="F18" s="12" t="s">
+    </row>
+    <row r="19" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B19" s="74"/>
+      <c r="C19" s="74"/>
+      <c r="D19" s="12" t="s">
         <v>90</v>
       </c>
-      <c r="G18" s="12" t="s">
+      <c r="E19" s="12" t="s">
+        <v>90</v>
+      </c>
+      <c r="F19" s="12" t="s">
+        <v>90</v>
+      </c>
+      <c r="G19" s="12" t="s">
+        <v>90</v>
+      </c>
+      <c r="H19" s="12" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="20" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B20" s="71"/>
+      <c r="C20" s="71"/>
+      <c r="D20" s="13" t="s">
         <v>91</v>
       </c>
-      <c r="H18" s="12" t="s">
+      <c r="E20" s="13" t="s">
+        <v>91</v>
+      </c>
+      <c r="F20" s="13" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="19" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B19" s="71"/>
-      <c r="C19" s="71"/>
-      <c r="D19" s="12" t="s">
+      <c r="G20" s="13" t="s">
         <v>93</v>
       </c>
-      <c r="E19" s="12" t="s">
+      <c r="H20" s="13" t="s">
         <v>93</v>
-      </c>
-      <c r="F19" s="12" t="s">
-        <v>93</v>
-      </c>
-      <c r="G19" s="12" t="s">
-        <v>93</v>
-      </c>
-      <c r="H19" s="12" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="20" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="72"/>
-      <c r="C20" s="72"/>
-      <c r="D20" s="13" t="s">
-        <v>94</v>
-      </c>
-      <c r="E20" s="13" t="s">
-        <v>94</v>
-      </c>
-      <c r="F20" s="13" t="s">
-        <v>95</v>
-      </c>
-      <c r="G20" s="13" t="s">
-        <v>96</v>
-      </c>
-      <c r="H20" s="13" t="s">
-        <v>96</v>
       </c>
     </row>
     <row r="21" spans="2:8" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -4020,84 +4068,84 @@
         <v>44</v>
       </c>
       <c r="C21" s="70" t="s">
+        <v>74</v>
+      </c>
+      <c r="D21" s="11" t="s">
+        <v>75</v>
+      </c>
+      <c r="E21" s="11" t="s">
+        <v>75</v>
+      </c>
+      <c r="F21" s="11" t="s">
+        <v>75</v>
+      </c>
+      <c r="G21" s="11" t="s">
+        <v>75</v>
+      </c>
+      <c r="H21" s="11" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="22" spans="2:8" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B22" s="74"/>
+      <c r="C22" s="74"/>
+      <c r="D22" s="11" t="s">
+        <v>76</v>
+      </c>
+      <c r="E22" s="11" t="s">
+        <v>76</v>
+      </c>
+      <c r="F22" s="11" t="s">
+        <v>76</v>
+      </c>
+      <c r="G22" s="11" t="s">
+        <v>76</v>
+      </c>
+      <c r="H22" s="11" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="23" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B23" s="74"/>
+      <c r="C23" s="74"/>
+      <c r="D23" s="11" t="s">
         <v>77</v>
       </c>
-      <c r="D21" s="11" t="s">
+      <c r="E23" s="11" t="s">
+        <v>77</v>
+      </c>
+      <c r="F23" s="11" t="s">
+        <v>77</v>
+      </c>
+      <c r="G23" s="11" t="s">
+        <v>77</v>
+      </c>
+      <c r="H23" s="11" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="24" spans="2:8" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B24" s="71"/>
+      <c r="C24" s="71"/>
+      <c r="D24" s="11" t="s">
+        <v>79</v>
+      </c>
+      <c r="E24" s="11" t="s">
         <v>78</v>
       </c>
-      <c r="E21" s="11" t="s">
+      <c r="F24" s="11" t="s">
         <v>78</v>
       </c>
-      <c r="F21" s="11" t="s">
-        <v>78</v>
-      </c>
-      <c r="G21" s="11" t="s">
-        <v>78</v>
-      </c>
-      <c r="H21" s="11" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="22" spans="2:8" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B22" s="71"/>
-      <c r="C22" s="71"/>
-      <c r="D22" s="11" t="s">
+      <c r="G24" s="11" t="s">
         <v>79</v>
       </c>
-      <c r="E22" s="11" t="s">
+      <c r="H24" s="11" t="s">
         <v>79</v>
-      </c>
-      <c r="F22" s="11" t="s">
-        <v>79</v>
-      </c>
-      <c r="G22" s="11" t="s">
-        <v>79</v>
-      </c>
-      <c r="H22" s="11" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="23" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B23" s="71"/>
-      <c r="C23" s="71"/>
-      <c r="D23" s="11" t="s">
-        <v>80</v>
-      </c>
-      <c r="E23" s="11" t="s">
-        <v>80</v>
-      </c>
-      <c r="F23" s="11" t="s">
-        <v>80</v>
-      </c>
-      <c r="G23" s="11" t="s">
-        <v>80</v>
-      </c>
-      <c r="H23" s="11" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="24" spans="2:8" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B24" s="72"/>
-      <c r="C24" s="72"/>
-      <c r="D24" s="11" t="s">
-        <v>82</v>
-      </c>
-      <c r="E24" s="11" t="s">
-        <v>81</v>
-      </c>
-      <c r="F24" s="11" t="s">
-        <v>81</v>
-      </c>
-      <c r="G24" s="11" t="s">
-        <v>82</v>
-      </c>
-      <c r="H24" s="11" t="s">
-        <v>82</v>
       </c>
     </row>
     <row r="25" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B25" s="15" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="C25" s="7"/>
       <c r="D25" s="7"/>
@@ -4108,24 +4156,24 @@
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="B14:B17"/>
+    <mergeCell ref="C14:C17"/>
+    <mergeCell ref="B18:B20"/>
+    <mergeCell ref="C18:C20"/>
+    <mergeCell ref="B21:B24"/>
+    <mergeCell ref="C21:C24"/>
+    <mergeCell ref="B4:B6"/>
+    <mergeCell ref="C4:C6"/>
+    <mergeCell ref="B7:B10"/>
+    <mergeCell ref="C7:C10"/>
+    <mergeCell ref="B11:B13"/>
+    <mergeCell ref="C11:C13"/>
     <mergeCell ref="H2:H3"/>
     <mergeCell ref="B2:B3"/>
     <mergeCell ref="D2:D3"/>
     <mergeCell ref="E2:E3"/>
     <mergeCell ref="F2:F3"/>
     <mergeCell ref="G2:G3"/>
-    <mergeCell ref="B4:B6"/>
-    <mergeCell ref="C4:C6"/>
-    <mergeCell ref="B7:B10"/>
-    <mergeCell ref="C7:C10"/>
-    <mergeCell ref="B11:B13"/>
-    <mergeCell ref="C11:C13"/>
-    <mergeCell ref="B14:B17"/>
-    <mergeCell ref="C14:C17"/>
-    <mergeCell ref="B18:B20"/>
-    <mergeCell ref="C18:C20"/>
-    <mergeCell ref="B21:B24"/>
-    <mergeCell ref="C21:C24"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>